<commit_message>
Daily attendance processing - 2026-02-09 11:03:54 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B1_session_analysis.xlsx
+++ b/attendance_reports/Y4_B2526_General_&_Special_Internal_1_B1_session_analysis.xlsx
@@ -484,7 +484,7 @@
     <col width="9" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="13" customWidth="1" min="7" max="7"/>
+    <col width="25" customWidth="1" min="7" max="7"/>
     <col width="10" customWidth="1" min="8" max="8"/>
     <col width="14" customWidth="1" min="9" max="9"/>
     <col width="22" customWidth="1" min="11" max="11"/>
@@ -2704,7 +2704,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G43" s="2" t="inlineStr"/>
+      <c r="G43" s="2" t="inlineStr">
+        <is>
+          <t>marinasamirxl@gmail.com</t>
+        </is>
+      </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
           <t>50/61</t>
@@ -2919,7 +2923,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G48" s="2" t="inlineStr"/>
+      <c r="G48" s="2" t="inlineStr">
+        <is>
+          <t>marinasamirxl@gmail.com</t>
+        </is>
+      </c>
       <c r="H48" s="2" t="inlineStr">
         <is>
           <t>54/61</t>
@@ -5155,7 +5163,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G100" s="2" t="inlineStr"/>
+      <c r="G100" s="2" t="inlineStr">
+        <is>
+          <t>marinasamirxl@gmail.com</t>
+        </is>
+      </c>
       <c r="H100" s="2" t="inlineStr">
         <is>
           <t>17/65</t>
@@ -7262,7 +7274,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G149" s="2" t="inlineStr"/>
+      <c r="G149" s="2" t="inlineStr">
+        <is>
+          <t>marinasamirxl@gmail.com</t>
+        </is>
+      </c>
       <c r="H149" s="2" t="inlineStr">
         <is>
           <t>53/63</t>
@@ -7391,7 +7407,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G152" s="2" t="inlineStr"/>
+      <c r="G152" s="2" t="inlineStr">
+        <is>
+          <t>marinasamirxl@gmail.com</t>
+        </is>
+      </c>
       <c r="H152" s="2" t="inlineStr">
         <is>
           <t>57/63</t>
@@ -9498,7 +9518,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G201" s="2" t="inlineStr"/>
+      <c r="G201" s="2" t="inlineStr">
+        <is>
+          <t>marinasamirxl@gmail.com</t>
+        </is>
+      </c>
       <c r="H201" s="2" t="inlineStr">
         <is>
           <t>57/66</t>
@@ -9627,7 +9651,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G204" s="2" t="inlineStr"/>
+      <c r="G204" s="2" t="inlineStr">
+        <is>
+          <t>marinasamirxl@gmail.com</t>
+        </is>
+      </c>
       <c r="H204" s="2" t="inlineStr">
         <is>
           <t>64/66</t>
@@ -9670,7 +9698,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G205" s="2" t="inlineStr"/>
+      <c r="G205" s="2" t="inlineStr">
+        <is>
+          <t>marinasamirxl@gmail.com</t>
+        </is>
+      </c>
       <c r="H205" s="2" t="inlineStr">
         <is>
           <t>20/66</t>
@@ -11691,7 +11723,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G252" s="2" t="inlineStr"/>
+      <c r="G252" s="2" t="inlineStr">
+        <is>
+          <t>marinasamirxl@gmail.com</t>
+        </is>
+      </c>
       <c r="H252" s="2" t="inlineStr">
         <is>
           <t>49/70</t>
@@ -11734,7 +11770,11 @@
           <t>09:00:00</t>
         </is>
       </c>
-      <c r="G253" s="2" t="inlineStr"/>
+      <c r="G253" s="2" t="inlineStr">
+        <is>
+          <t>marinasamirxl@gmail.com</t>
+        </is>
+      </c>
       <c r="H253" s="2" t="inlineStr">
         <is>
           <t>36/70</t>

</xml_diff>